<commit_message>
more consolidation and cleanup
</commit_message>
<xml_diff>
--- a/argot/working_docs/endeca_fields_to_Argot.xlsx
+++ b/argot/working_docs/endeca_fields_to_Argot.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="164">
   <si>
     <t>Element name</t>
   </si>
@@ -43,18 +43,6 @@
     <t>yes</t>
   </si>
   <si>
-    <t>Access Restrictions</t>
-  </si>
-  <si>
-    <t>Access Restriction</t>
-  </si>
-  <si>
-    <t>Biographical Sketch</t>
-  </si>
-  <si>
-    <t>Keyword, Keyword_Brief</t>
-  </si>
-  <si>
     <t>Cartographic Data</t>
   </si>
   <si>
@@ -64,36 +52,15 @@
     <t>Collective Uniform Title</t>
   </si>
   <si>
-    <t>Constituent Unit Linking</t>
-  </si>
-  <si>
-    <t>Current Frequency</t>
-  </si>
-  <si>
     <t>Author, Author_Brief, Keyword, Keyword_Brief</t>
   </si>
   <si>
-    <t>Donor</t>
-  </si>
-  <si>
-    <t>Earlier Title</t>
-  </si>
-  <si>
     <t>Keyword, Keyword_Brief, Title</t>
   </si>
   <si>
     <t>Format</t>
   </si>
   <si>
-    <t>Former Frequency</t>
-  </si>
-  <si>
-    <t>Has Supplement Linking</t>
-  </si>
-  <si>
-    <t>Host Item Linking</t>
-  </si>
-  <si>
     <t>ICE Chapter Title</t>
   </si>
   <si>
@@ -106,24 +73,12 @@
     <t>ISBN, Keyword</t>
   </si>
   <si>
-    <t>ISSN</t>
-  </si>
-  <si>
     <t>Journal_Concise, Journal_Title</t>
   </si>
   <si>
     <t>Journal Title Abbreviation</t>
   </si>
   <si>
-    <t>Later Title</t>
-  </si>
-  <si>
-    <t>Linking ISSN</t>
-  </si>
-  <si>
-    <t>Linking_ISSN</t>
-  </si>
-  <si>
     <t>LocalId</t>
   </si>
   <si>
@@ -136,9 +91,6 @@
     <t>Main Uniform Title</t>
   </si>
   <si>
-    <t>Material</t>
-  </si>
-  <si>
     <t>Material Details</t>
   </si>
   <si>
@@ -163,15 +115,9 @@
     <t>Author, Keyword, Keyword_Brief</t>
   </si>
   <si>
-    <t>Other Edition</t>
-  </si>
-  <si>
     <t>Other Title Translation</t>
   </si>
   <si>
-    <t>Other Titles</t>
-  </si>
-  <si>
     <t>Performer Credits</t>
   </si>
   <si>
@@ -181,9 +127,6 @@
     <t>PubDateSort</t>
   </si>
   <si>
-    <t>Related Collections</t>
-  </si>
-  <si>
     <t>Series</t>
   </si>
   <si>
@@ -193,33 +136,18 @@
     <t>Series Statement</t>
   </si>
   <si>
-    <t>Source of Acquisition</t>
-  </si>
-  <si>
     <t>Subseries Linking</t>
   </si>
   <si>
-    <t>Supplement to Linking</t>
-  </si>
-  <si>
     <t>Syndetics ISBN</t>
   </si>
   <si>
     <t>Syndetics_ISBN</t>
   </si>
   <si>
-    <t>System Details</t>
-  </si>
-  <si>
     <t>Title Index</t>
   </si>
   <si>
-    <t>Translated as Linking</t>
-  </si>
-  <si>
-    <t>Translation of Linking</t>
-  </si>
-  <si>
     <t>UPC</t>
   </si>
   <si>
@@ -232,12 +160,6 @@
     <t>Argot field</t>
   </si>
   <si>
-    <t>note_access_restriction</t>
-  </si>
-  <si>
-    <t>For details in Endeca, see "By MARC tag &gt; 545" section of https://docs.google.com/document/d/1Yh1DoDWpJ00e_DCQQyZFmAjC71htAP99t5jjEt_03fQ/edit?usp=sharing</t>
-  </si>
-  <si>
     <t>Argot display</t>
   </si>
   <si>
@@ -247,24 +169,9 @@
     <t>n</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>na</t>
   </si>
   <si>
-    <t>note_biographical</t>
-  </si>
-  <si>
-    <t>included_work</t>
-  </si>
-  <si>
-    <t>related_work</t>
-  </si>
-  <si>
-    <t>misc_id</t>
-  </si>
-  <si>
     <t>Label</t>
   </si>
   <si>
@@ -277,18 +184,9 @@
     <t>Title portion indexed in indexed-only title_uniform.  Author portion indexed in author_main. Stored for display and creation of hyperlink</t>
   </si>
   <si>
-    <t>Related works section?</t>
-  </si>
-  <si>
     <t>These are indexed only titles, including variants coded as index-only in 246, abbreviated title</t>
   </si>
   <si>
-    <t>note_title_complexity</t>
-  </si>
-  <si>
-    <t>Display only. Indexed in index-only related_author and related_title fields</t>
-  </si>
-  <si>
     <t>resource_type</t>
   </si>
   <si>
@@ -298,12 +196,6 @@
     <t>Facet values, but should also probably display on each record</t>
   </si>
   <si>
-    <t>frequency[current]</t>
-  </si>
-  <si>
-    <t>frequency[former]</t>
-  </si>
-  <si>
     <t>series_transcribed</t>
   </si>
   <si>
@@ -331,72 +223,18 @@
     <t>indexed</t>
   </si>
   <si>
-    <t>donor</t>
-  </si>
-  <si>
-    <t>author; keyword</t>
-  </si>
-  <si>
-    <t>IDs &gt; ISSN:</t>
-  </si>
-  <si>
-    <t>ids</t>
-  </si>
-  <si>
-    <t>Related works &gt; Continued by:</t>
-  </si>
-  <si>
-    <t>title_related; keyword</t>
-  </si>
-  <si>
-    <t>Label may vary, as specified in MARC coding</t>
-  </si>
-  <si>
-    <t>keyword</t>
-  </si>
-  <si>
-    <t>Related works</t>
-  </si>
-  <si>
-    <t>Included works</t>
-  </si>
-  <si>
-    <t>title_included; author_included; keyword</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Related works &gt; Supplement: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Related works &gt; Part of: </t>
-  </si>
-  <si>
     <t>Related works &gt; Other versions of this work</t>
   </si>
   <si>
     <t>title; author; keyword</t>
   </si>
   <si>
-    <t>title_related; author; keyword</t>
-  </si>
-  <si>
     <t>titles_included_ice</t>
   </si>
   <si>
     <t>Display is provided by Syndetics API at load time</t>
   </si>
   <si>
-    <t xml:space="preserve">Notes &gt; Acquisition details: </t>
-  </si>
-  <si>
-    <t>Donor name should be in indexed in donor field</t>
-  </si>
-  <si>
-    <t>genre_headings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adaptive hyperlinking, like subjects. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Mapped from 242c in Endeca. Used in 2 bib records at UNC. How much do we care about this? </t>
   </si>
   <si>
@@ -427,12 +265,6 @@
     <t>local_id[value]</t>
   </si>
   <si>
-    <t>physical_description</t>
-  </si>
-  <si>
-    <t>currently mapped to argot as 'description[general]'</t>
-  </si>
-  <si>
     <t>musical_presentation_statement</t>
   </si>
   <si>
@@ -460,9 +292,6 @@
     <t>defer for shared records</t>
   </si>
   <si>
-    <t>note_acquisition_source</t>
-  </si>
-  <si>
     <t>syndetics_id</t>
   </si>
   <si>
@@ -475,15 +304,9 @@
     <t>ticket</t>
   </si>
   <si>
-    <t>https://trlnmain.atlassian.net/browse/TD-461</t>
-  </si>
-  <si>
     <t>https://trlnmain.atlassian.net/browse/TD-462</t>
   </si>
   <si>
-    <t>https://trlnmain.atlassian.net/browse/TD-463</t>
-  </si>
-  <si>
     <t>https://trlnmain.atlassian.net/browse/TD-442</t>
   </si>
   <si>
@@ -508,12 +331,6 @@
     <t>https://trlnmain.atlassian.net/browse/TD-435</t>
   </si>
   <si>
-    <t>https://trlnmain.atlassian.net/browse/TD-468</t>
-  </si>
-  <si>
-    <t>https://trlnmain.atlassian.net/browse/TD-469</t>
-  </si>
-  <si>
     <t>https://trlnmain.atlassian.net/browse/TD-160</t>
   </si>
   <si>
@@ -553,18 +370,12 @@
     <t>https://trlnmain.atlassian.net/browse/TD-482</t>
   </si>
   <si>
-    <t>note_display</t>
-  </si>
-  <si>
     <t>subject_heading_mesh</t>
   </si>
   <si>
     <t>https://trlnmain.atlassian.net/browse/TD-131</t>
   </si>
   <si>
-    <t>note_display; note_index</t>
-  </si>
-  <si>
     <t>document - done in spreadsheet.</t>
   </si>
   <si>
@@ -580,12 +391,6 @@
     <t>https://trlnmain.atlassian.net/browse/TD-493</t>
   </si>
   <si>
-    <t>https://trlnmain.atlassian.net/browse/TD-134</t>
-  </si>
-  <si>
-    <t>The locations of other related archival etc. collections</t>
-  </si>
-  <si>
     <t>series; title; keyword</t>
   </si>
   <si>
@@ -598,12 +403,6 @@
     <t>tbd</t>
   </si>
   <si>
-    <t>related_work_earlier</t>
-  </si>
-  <si>
-    <t>related_work_later</t>
-  </si>
-  <si>
     <t>Column(s)</t>
   </si>
   <si>
@@ -694,9 +493,6 @@
     <t xml:space="preserve">This is based on the set of all Endeca property and dimensions that were not already mapped into Argot when I began this work. </t>
   </si>
   <si>
-    <t>Notes &gt; Biographical sketch:</t>
-  </si>
-  <si>
     <t>Related items &gt; ??</t>
   </si>
   <si>
@@ -716,18 +512,6 @@
   </si>
   <si>
     <t>Other details &gt; (material description cluster) &gt; Cartographic details:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other details &gt; (copy/institution specific cluster) &gt; Donor: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other details &gt; (continuing resources-specific cluster) &gt; Frequency: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other details &gt; (continuing resources-specific cluster) &gt; Former frequency: </t>
-  </si>
-  <si>
-    <t>"This item is about" is not accurate</t>
   </si>
 </sst>
 </file>
@@ -1220,9 +1004,8 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1343,8 +1126,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="endecafields" displayName="endecafields" ref="A1:M59" totalsRowShown="0">
-  <autoFilter ref="A1:M59"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="endecafields" displayName="endecafields" ref="A1:M33" totalsRowShown="0">
+  <autoFilter ref="A1:M33"/>
   <tableColumns count="13">
     <tableColumn id="1" name="Element name"/>
     <tableColumn id="2" name="Endeca dmod name"/>
@@ -1636,221 +1419,221 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.42578125" customWidth="1"/>
-    <col min="2" max="2" width="65.28515625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="65.28515625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="B1" s="3"/>
+      <c r="A1" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B1" s="2"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>194</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>195</v>
+        <v>127</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>196</v>
+      <c r="B4" s="3" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>197</v>
+      <c r="B5" s="3" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>198</v>
+      <c r="B6" s="3" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>199</v>
+      <c r="B7" s="3" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>200</v>
+      <c r="A8" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>201</v>
+      <c r="A9" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>202</v>
+      <c r="A10" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>203</v>
+      <c r="A11" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>204</v>
+      <c r="A12" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>206</v>
+      <c r="A13" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>205</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>207</v>
+      <c r="A14" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>208</v>
+      <c r="A15" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>209</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>210</v>
+        <v>142</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>211</v>
+      <c r="A19" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>212</v>
+      <c r="A20" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>213</v>
+      <c r="A21" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>214</v>
+      <c r="A22" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>215</v>
+      <c r="A23" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>216</v>
+      <c r="A24" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>218</v>
+      <c r="A25" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>217</v>
+      <c r="A26" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>219</v>
+      <c r="A27" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>220</v>
+      <c r="A28" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>221</v>
+      <c r="A29" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>222</v>
+      <c r="A30" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -1867,10 +1650,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M59"/>
+  <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A15" sqref="A15:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1897,80 +1680,80 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="F1" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c r="G1" t="s">
-        <v>72</v>
+        <v>46</v>
       </c>
       <c r="H1" t="s">
-        <v>81</v>
+        <v>50</v>
       </c>
       <c r="I1" t="s">
-        <v>226</v>
+        <v>158</v>
       </c>
       <c r="J1" t="s">
-        <v>102</v>
+        <v>66</v>
       </c>
       <c r="K1" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="L1" t="s">
-        <v>205</v>
+        <v>138</v>
       </c>
       <c r="M1" t="s">
-        <v>150</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="F2" t="s">
-        <v>134</v>
+        <v>80</v>
       </c>
       <c r="G2" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="H2" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="I2" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="J2" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="K2" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="L2" t="s">
-        <v>129</v>
+        <v>75</v>
       </c>
       <c r="M2" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -1979,39 +1762,39 @@
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="F3" t="s">
-        <v>142</v>
+        <v>86</v>
       </c>
       <c r="G3" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="H3" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="I3" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="J3" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="K3" t="s">
-        <v>143</v>
+        <v>87</v>
       </c>
       <c r="L3" t="s">
-        <v>129</v>
+        <v>75</v>
       </c>
       <c r="M3" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -2020,80 +1803,80 @@
         <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>74</v>
+        <v>48</v>
       </c>
       <c r="F4" t="s">
-        <v>147</v>
+        <v>90</v>
       </c>
       <c r="G4" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="H4" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="I4" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="J4" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="K4" t="s">
-        <v>148</v>
+        <v>91</v>
       </c>
       <c r="L4" t="s">
-        <v>129</v>
+        <v>75</v>
       </c>
       <c r="M4" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="F5" t="s">
-        <v>101</v>
+        <v>65</v>
       </c>
       <c r="G5" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="H5" t="s">
-        <v>231</v>
+        <v>163</v>
       </c>
       <c r="I5" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="J5" t="s">
         <v>5</v>
       </c>
       <c r="K5" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="L5" t="s">
-        <v>126</v>
+        <v>72</v>
       </c>
       <c r="M5" t="s">
-        <v>152</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -2102,39 +1885,39 @@
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="F6" t="s">
-        <v>172</v>
+        <v>111</v>
       </c>
       <c r="G6" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="H6" t="s">
-        <v>230</v>
+        <v>162</v>
       </c>
       <c r="I6" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="J6" t="s">
         <v>5</v>
       </c>
       <c r="K6" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="L6" t="s">
-        <v>126</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>176</v>
+        <v>72</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -2143,39 +1926,39 @@
         <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="F7" t="s">
-        <v>170</v>
+        <v>109</v>
       </c>
       <c r="G7" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="H7" t="s">
-        <v>229</v>
+        <v>161</v>
       </c>
       <c r="I7" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="J7" t="s">
         <v>5</v>
       </c>
       <c r="K7" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="L7" t="s">
-        <v>126</v>
+        <v>72</v>
       </c>
       <c r="M7" t="s">
-        <v>174</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -2184,39 +1967,39 @@
         <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="F8" t="s">
-        <v>169</v>
+        <v>108</v>
       </c>
       <c r="G8" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="H8" t="s">
-        <v>228</v>
+        <v>160</v>
       </c>
       <c r="I8" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="J8" t="s">
         <v>5</v>
       </c>
       <c r="K8" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="L8" t="s">
-        <v>126</v>
+        <v>72</v>
       </c>
       <c r="M8" t="s">
-        <v>173</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -2225,80 +2008,80 @@
         <v>5</v>
       </c>
       <c r="E9" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="F9" t="s">
-        <v>171</v>
+        <v>110</v>
       </c>
       <c r="G9" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="H9" t="s">
-        <v>227</v>
+        <v>159</v>
       </c>
       <c r="I9" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="J9" t="s">
         <v>5</v>
       </c>
       <c r="K9" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="L9" t="s">
-        <v>126</v>
+        <v>72</v>
       </c>
       <c r="M9" t="s">
-        <v>175</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E10" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="F10" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="G10" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="H10" t="s">
-        <v>232</v>
+        <v>64</v>
       </c>
       <c r="I10" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="J10" t="s">
-        <v>104</v>
+        <v>64</v>
       </c>
       <c r="K10" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="L10" t="s">
-        <v>126</v>
+        <v>72</v>
       </c>
       <c r="M10" t="s">
-        <v>151</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -2307,326 +2090,326 @@
         <v>5</v>
       </c>
       <c r="E11" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="F11" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="G11" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="H11" t="s">
-        <v>233</v>
+        <v>64</v>
       </c>
       <c r="I11" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="J11" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="K11" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="L11" t="s">
-        <v>126</v>
+        <v>72</v>
       </c>
       <c r="M11" t="s">
-        <v>153</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E12" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="F12" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="G12" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="H12" t="s">
-        <v>234</v>
+        <v>64</v>
       </c>
       <c r="I12" t="s">
+        <v>64</v>
+      </c>
+      <c r="J12" t="s">
+        <v>64</v>
+      </c>
+      <c r="K12" t="s">
+        <v>64</v>
+      </c>
+      <c r="L12" t="s">
+        <v>72</v>
+      </c>
+      <c r="M12" t="s">
         <v>100</v>
-      </c>
-      <c r="J12" t="s">
-        <v>100</v>
-      </c>
-      <c r="K12" t="s">
-        <v>100</v>
-      </c>
-      <c r="L12" t="s">
-        <v>126</v>
-      </c>
-      <c r="M12" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>100</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>100</v>
+        <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>100</v>
+        <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>100</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>100</v>
+        <v>5</v>
+      </c>
+      <c r="E13" t="s">
+        <v>48</v>
       </c>
       <c r="F13" t="s">
-        <v>123</v>
+        <v>56</v>
       </c>
       <c r="G13" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="H13" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="I13" t="s">
-        <v>235</v>
+        <v>64</v>
       </c>
       <c r="J13" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="K13" t="s">
-        <v>124</v>
+        <v>57</v>
       </c>
       <c r="L13" t="s">
-        <v>126</v>
+        <v>72</v>
       </c>
       <c r="M13" t="s">
-        <v>163</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E14" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="F14" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="G14" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="H14" t="s">
-        <v>112</v>
+        <v>64</v>
       </c>
       <c r="I14" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="J14" t="s">
-        <v>113</v>
+        <v>64</v>
       </c>
       <c r="K14" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="L14" t="s">
-        <v>126</v>
+        <v>72</v>
       </c>
       <c r="M14" t="s">
-        <v>154</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D15" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="E15" t="s">
-        <v>73</v>
+        <v>48</v>
       </c>
       <c r="F15" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="G15" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="H15" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="I15" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="J15" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="K15" t="s">
-        <v>100</v>
+        <v>57</v>
       </c>
       <c r="L15" t="s">
-        <v>126</v>
+        <v>72</v>
       </c>
       <c r="M15" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>100</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>74</v>
+        <v>5</v>
+      </c>
+      <c r="E16" t="s">
+        <v>47</v>
       </c>
       <c r="F16" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="G16" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="H16" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="I16" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="J16" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="K16" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="L16" t="s">
-        <v>126</v>
+        <v>72</v>
       </c>
       <c r="M16" t="s">
-        <v>154</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="E17" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="F17" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="G17" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="H17" t="s">
-        <v>105</v>
+        <v>61</v>
       </c>
       <c r="I17" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="J17" t="s">
-        <v>106</v>
+        <v>64</v>
       </c>
       <c r="K17" t="s">
-        <v>100</v>
+        <v>63</v>
       </c>
       <c r="L17" t="s">
-        <v>126</v>
+        <v>72</v>
       </c>
       <c r="M17" t="s">
-        <v>186</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B18" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="E18" t="s">
-        <v>74</v>
+        <v>47</v>
       </c>
       <c r="F18" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="G18" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="H18" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="I18" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="J18" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="K18" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="L18" t="s">
-        <v>126</v>
+        <v>72</v>
       </c>
       <c r="M18" t="s">
-        <v>186</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
@@ -2635,1671 +2418,605 @@
         <v>5</v>
       </c>
       <c r="E19" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="F19" t="s">
-        <v>137</v>
+        <v>58</v>
       </c>
       <c r="G19" t="s">
-        <v>100</v>
+        <v>47</v>
       </c>
       <c r="H19" t="s">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="I19" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="J19" t="s">
-        <v>100</v>
+        <v>123</v>
       </c>
       <c r="K19" t="s">
-        <v>100</v>
+        <v>62</v>
       </c>
       <c r="L19" t="s">
-        <v>126</v>
+        <v>72</v>
       </c>
       <c r="M19" t="s">
-        <v>168</v>
+        <v>97</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="B20" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E20" t="s">
-        <v>73</v>
+        <v>48</v>
       </c>
       <c r="F20" t="s">
-        <v>70</v>
+        <v>88</v>
       </c>
       <c r="G20" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="H20" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="I20" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="J20" t="s">
-        <v>5</v>
+        <v>64</v>
       </c>
       <c r="K20" t="s">
-        <v>100</v>
+        <v>124</v>
       </c>
       <c r="L20" t="s">
-        <v>126</v>
+        <v>72</v>
       </c>
       <c r="M20" t="s">
-        <v>164</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="B21" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="E21" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="F21" t="s">
-        <v>146</v>
+        <v>83</v>
       </c>
       <c r="G21" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="H21" t="s">
-        <v>121</v>
+        <v>64</v>
       </c>
       <c r="I21" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="J21" t="s">
-        <v>5</v>
+        <v>64</v>
       </c>
       <c r="K21" t="s">
+        <v>71</v>
+      </c>
+      <c r="L21" t="s">
+        <v>72</v>
+      </c>
+      <c r="M21" t="s">
         <v>122</v>
-      </c>
-      <c r="L21" t="s">
-        <v>126</v>
-      </c>
-      <c r="M21" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="C22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D22" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E22" t="s">
-        <v>73</v>
+        <v>48</v>
       </c>
       <c r="F22" t="s">
-        <v>77</v>
+        <v>116</v>
       </c>
       <c r="G22" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="H22" t="s">
-        <v>224</v>
+        <v>64</v>
       </c>
       <c r="I22" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="J22" t="s">
-        <v>110</v>
+        <v>64</v>
       </c>
       <c r="K22" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="L22" t="s">
-        <v>126</v>
+        <v>72</v>
       </c>
       <c r="M22" t="s">
-        <v>164</v>
+        <v>117</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>62</v>
+        <v>14</v>
       </c>
       <c r="B23" t="s">
-        <v>62</v>
+        <v>14</v>
       </c>
       <c r="C23" t="s">
         <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E23" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="F23" t="s">
-        <v>177</v>
+        <v>126</v>
       </c>
       <c r="G23" t="s">
-        <v>100</v>
+        <v>47</v>
       </c>
       <c r="H23" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="I23" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="J23" t="s">
-        <v>100</v>
-      </c>
-      <c r="K23">
-        <v>538</v>
+        <v>64</v>
+      </c>
+      <c r="K23" t="s">
+        <v>77</v>
       </c>
       <c r="L23" t="s">
-        <v>126</v>
+        <v>72</v>
       </c>
       <c r="M23" t="s">
-        <v>164</v>
+        <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="B24" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E24" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="F24" t="s">
-        <v>180</v>
+        <v>126</v>
       </c>
       <c r="G24" t="s">
-        <v>100</v>
+        <v>47</v>
       </c>
       <c r="H24" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="I24" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="J24" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="K24" t="s">
-        <v>187</v>
+        <v>77</v>
       </c>
       <c r="L24" t="s">
-        <v>126</v>
+        <v>72</v>
       </c>
       <c r="M24" t="s">
-        <v>164</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="B25" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
       </c>
       <c r="D25" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="E25" t="s">
-        <v>73</v>
+        <v>48</v>
       </c>
       <c r="F25" t="s">
-        <v>87</v>
+        <v>51</v>
       </c>
       <c r="G25" t="s">
-        <v>73</v>
+        <v>48</v>
       </c>
       <c r="H25" t="s">
-        <v>111</v>
+        <v>64</v>
       </c>
       <c r="I25" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="J25" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="K25" t="s">
-        <v>88</v>
+        <v>54</v>
       </c>
       <c r="L25" t="s">
-        <v>126</v>
+        <v>72</v>
       </c>
       <c r="M25" t="s">
-        <v>164</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B26" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C26" t="s">
         <v>4</v>
       </c>
       <c r="D26" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E26" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="F26" t="s">
-        <v>138</v>
+        <v>51</v>
       </c>
       <c r="G26" t="s">
-        <v>100</v>
+        <v>48</v>
       </c>
       <c r="H26" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="I26" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="J26" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="K26" t="s">
-        <v>100</v>
+        <v>54</v>
       </c>
       <c r="L26" t="s">
-        <v>126</v>
+        <v>72</v>
       </c>
       <c r="M26" t="s">
-        <v>167</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B27" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C27" t="s">
         <v>4</v>
       </c>
       <c r="D27" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E27" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="F27" t="s">
-        <v>140</v>
+        <v>51</v>
       </c>
       <c r="G27" t="s">
-        <v>100</v>
+        <v>48</v>
       </c>
       <c r="H27" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="I27" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="J27" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="K27" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="L27" t="s">
-        <v>126</v>
+        <v>72</v>
       </c>
       <c r="M27" t="s">
-        <v>159</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B28" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E28" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="F28" t="s">
-        <v>135</v>
+        <v>52</v>
       </c>
       <c r="G28" t="s">
-        <v>100</v>
+        <v>47</v>
       </c>
       <c r="H28" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="I28" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="J28" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="K28" t="s">
-        <v>136</v>
+        <v>64</v>
       </c>
       <c r="L28" t="s">
-        <v>126</v>
+        <v>72</v>
       </c>
       <c r="M28" t="s">
-        <v>162</v>
+        <v>104</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="B29" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="C29" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D29" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="E29" t="s">
-        <v>74</v>
+        <v>47</v>
       </c>
       <c r="F29" t="s">
-        <v>90</v>
+        <v>52</v>
       </c>
       <c r="G29" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="H29" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="I29" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="J29" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="K29" t="s">
-        <v>91</v>
+        <v>64</v>
       </c>
       <c r="L29" t="s">
-        <v>126</v>
+        <v>72</v>
       </c>
       <c r="M29" t="s">
-        <v>161</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>51</v>
+        <v>13</v>
       </c>
       <c r="B30" t="s">
-        <v>51</v>
+        <v>13</v>
       </c>
       <c r="C30" t="s">
         <v>4</v>
       </c>
       <c r="D30" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E30" t="s">
-        <v>73</v>
+        <v>48</v>
       </c>
       <c r="F30" t="s">
-        <v>141</v>
+        <v>69</v>
       </c>
       <c r="G30" t="s">
-        <v>100</v>
+        <v>48</v>
       </c>
       <c r="H30" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="I30" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="J30" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="K30" t="s">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="L30" t="s">
-        <v>126</v>
+        <v>72</v>
       </c>
       <c r="M30" t="s">
-        <v>160</v>
+        <v>105</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="B31" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="C31" t="s">
         <v>4</v>
       </c>
       <c r="D31" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E31" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="F31" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="G31" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="H31" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="I31" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="J31" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="K31" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="L31" t="s">
-        <v>126</v>
+        <v>72</v>
       </c>
       <c r="M31" t="s">
-        <v>154</v>
+        <v>98</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="B32" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="C32" t="s">
         <v>4</v>
       </c>
       <c r="D32" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E32" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="F32" t="s">
-        <v>79</v>
+        <v>121</v>
       </c>
       <c r="G32" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="H32" t="s">
-        <v>115</v>
+        <v>157</v>
       </c>
       <c r="I32" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="J32" t="s">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="K32" t="s">
-        <v>100</v>
+        <v>53</v>
       </c>
       <c r="L32" t="s">
-        <v>126</v>
+        <v>72</v>
       </c>
       <c r="M32" t="s">
-        <v>154</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="B33" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="C33" t="s">
         <v>4</v>
       </c>
       <c r="D33" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="E33" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="F33" t="s">
-        <v>79</v>
+        <v>121</v>
       </c>
       <c r="G33" t="s">
-        <v>100</v>
+        <v>47</v>
       </c>
       <c r="H33" t="s">
-        <v>100</v>
+        <v>67</v>
       </c>
       <c r="I33" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="J33" t="s">
-        <v>100</v>
+        <v>68</v>
       </c>
       <c r="K33" t="s">
-        <v>100</v>
+        <v>53</v>
       </c>
       <c r="L33" t="s">
-        <v>126</v>
+        <v>72</v>
       </c>
       <c r="M33" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>59</v>
-      </c>
-      <c r="B34" t="s">
-        <v>59</v>
-      </c>
-      <c r="C34" t="s">
-        <v>4</v>
-      </c>
-      <c r="D34" t="s">
-        <v>5</v>
-      </c>
-      <c r="E34" t="s">
-        <v>73</v>
-      </c>
-      <c r="F34" t="s">
-        <v>79</v>
-      </c>
-      <c r="G34" t="s">
-        <v>100</v>
-      </c>
-      <c r="H34" t="s">
-        <v>100</v>
-      </c>
-      <c r="I34" t="s">
-        <v>100</v>
-      </c>
-      <c r="J34" t="s">
-        <v>100</v>
-      </c>
-      <c r="K34" t="s">
-        <v>100</v>
-      </c>
-      <c r="L34" t="s">
-        <v>126</v>
-      </c>
-      <c r="M34" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>64</v>
-      </c>
-      <c r="B35" t="s">
-        <v>64</v>
-      </c>
-      <c r="C35" t="s">
-        <v>4</v>
-      </c>
-      <c r="D35" t="s">
-        <v>10</v>
-      </c>
-      <c r="E35" t="s">
-        <v>73</v>
-      </c>
-      <c r="F35" t="s">
-        <v>79</v>
-      </c>
-      <c r="G35" t="s">
-        <v>100</v>
-      </c>
-      <c r="H35" t="s">
-        <v>100</v>
-      </c>
-      <c r="I35" t="s">
-        <v>100</v>
-      </c>
-      <c r="J35" t="s">
-        <v>100</v>
-      </c>
-      <c r="K35" t="s">
-        <v>100</v>
-      </c>
-      <c r="L35" t="s">
-        <v>126</v>
-      </c>
-      <c r="M35" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>65</v>
-      </c>
-      <c r="B36" t="s">
-        <v>65</v>
-      </c>
-      <c r="C36" t="s">
-        <v>4</v>
-      </c>
-      <c r="D36" t="s">
-        <v>10</v>
-      </c>
-      <c r="E36" t="s">
-        <v>73</v>
-      </c>
-      <c r="F36" t="s">
-        <v>79</v>
-      </c>
-      <c r="G36" t="s">
-        <v>100</v>
-      </c>
-      <c r="H36" t="s">
-        <v>100</v>
-      </c>
-      <c r="I36" t="s">
-        <v>100</v>
-      </c>
-      <c r="J36" t="s">
-        <v>100</v>
-      </c>
-      <c r="K36" t="s">
-        <v>100</v>
-      </c>
-      <c r="L36" t="s">
-        <v>126</v>
-      </c>
-      <c r="M36" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>100</v>
-      </c>
-      <c r="B37" t="s">
-        <v>100</v>
-      </c>
-      <c r="C37" t="s">
-        <v>100</v>
-      </c>
-      <c r="D37" t="s">
-        <v>100</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F37" t="s">
-        <v>79</v>
-      </c>
-      <c r="G37" t="s">
-        <v>73</v>
-      </c>
-      <c r="H37" t="s">
-        <v>111</v>
-      </c>
-      <c r="I37" t="s">
-        <v>100</v>
-      </c>
-      <c r="J37" t="s">
-        <v>118</v>
-      </c>
-      <c r="K37" t="s">
-        <v>100</v>
-      </c>
-      <c r="L37" t="s">
-        <v>126</v>
-      </c>
-      <c r="M37" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>100</v>
-      </c>
-      <c r="B38" t="s">
-        <v>49</v>
-      </c>
-      <c r="C38" t="s">
-        <v>4</v>
-      </c>
-      <c r="D38" t="s">
-        <v>19</v>
-      </c>
-      <c r="E38" t="s">
-        <v>73</v>
-      </c>
-      <c r="F38" t="s">
-        <v>79</v>
-      </c>
-      <c r="G38" t="s">
-        <v>73</v>
-      </c>
-      <c r="H38" t="s">
-        <v>100</v>
-      </c>
-      <c r="I38" t="s">
-        <v>100</v>
-      </c>
-      <c r="J38" t="s">
-        <v>100</v>
-      </c>
-      <c r="K38" t="s">
-        <v>100</v>
-      </c>
-      <c r="L38" t="s">
-        <v>126</v>
-      </c>
-      <c r="M38" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>18</v>
-      </c>
-      <c r="B39" t="s">
-        <v>18</v>
-      </c>
-      <c r="C39" t="s">
-        <v>4</v>
-      </c>
-      <c r="D39" t="s">
-        <v>19</v>
-      </c>
-      <c r="E39" t="s">
-        <v>73</v>
-      </c>
-      <c r="F39" t="s">
-        <v>192</v>
-      </c>
-      <c r="G39" t="s">
-        <v>73</v>
-      </c>
-      <c r="H39" t="s">
-        <v>85</v>
-      </c>
-      <c r="I39" t="s">
-        <v>100</v>
-      </c>
-      <c r="J39" t="s">
-        <v>100</v>
-      </c>
-      <c r="K39" t="s">
-        <v>100</v>
-      </c>
-      <c r="L39" t="s">
-        <v>126</v>
-      </c>
-      <c r="M39" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>31</v>
-      </c>
-      <c r="B40" t="s">
-        <v>31</v>
-      </c>
-      <c r="C40" t="s">
-        <v>4</v>
-      </c>
-      <c r="D40" t="s">
-        <v>19</v>
-      </c>
-      <c r="E40" t="s">
-        <v>73</v>
-      </c>
-      <c r="F40" t="s">
-        <v>193</v>
-      </c>
-      <c r="G40" t="s">
-        <v>73</v>
-      </c>
-      <c r="H40" t="s">
-        <v>107</v>
-      </c>
-      <c r="I40" t="s">
-        <v>100</v>
-      </c>
-      <c r="J40" t="s">
-        <v>108</v>
-      </c>
-      <c r="K40" t="s">
-        <v>109</v>
-      </c>
-      <c r="L40" t="s">
-        <v>126</v>
-      </c>
-      <c r="M40" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>20</v>
-      </c>
-      <c r="B41" t="s">
-        <v>20</v>
-      </c>
-      <c r="C41" t="s">
-        <v>6</v>
-      </c>
-      <c r="D41" t="s">
-        <v>5</v>
-      </c>
-      <c r="E41" t="s">
-        <v>74</v>
-      </c>
-      <c r="F41" t="s">
-        <v>89</v>
-      </c>
-      <c r="G41" t="s">
-        <v>73</v>
-      </c>
-      <c r="H41" t="s">
-        <v>100</v>
-      </c>
-      <c r="I41" t="s">
-        <v>100</v>
-      </c>
-      <c r="J41" t="s">
-        <v>100</v>
-      </c>
-      <c r="K41" t="s">
-        <v>91</v>
-      </c>
-      <c r="L41" t="s">
-        <v>126</v>
-      </c>
-      <c r="M41" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>35</v>
-      </c>
-      <c r="B42" t="s">
-        <v>35</v>
-      </c>
-      <c r="C42" t="s">
-        <v>4</v>
-      </c>
-      <c r="D42" t="s">
-        <v>5</v>
-      </c>
-      <c r="E42" t="s">
-        <v>73</v>
-      </c>
-      <c r="F42" t="s">
-        <v>95</v>
-      </c>
-      <c r="G42" t="s">
-        <v>100</v>
-      </c>
-      <c r="H42" t="s">
-        <v>100</v>
-      </c>
-      <c r="I42" t="s">
-        <v>100</v>
-      </c>
-      <c r="J42" t="s">
-        <v>100</v>
-      </c>
-      <c r="K42" t="s">
-        <v>100</v>
-      </c>
-      <c r="L42" t="s">
-        <v>126</v>
-      </c>
-      <c r="M42" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>56</v>
-      </c>
-      <c r="B43" t="s">
-        <v>56</v>
-      </c>
-      <c r="C43" t="s">
-        <v>4</v>
-      </c>
-      <c r="D43" t="s">
-        <v>19</v>
-      </c>
-      <c r="E43" t="s">
-        <v>73</v>
-      </c>
-      <c r="F43" t="s">
-        <v>95</v>
-      </c>
-      <c r="G43" t="s">
-        <v>73</v>
-      </c>
-      <c r="H43" t="s">
-        <v>97</v>
-      </c>
-      <c r="I43" t="s">
-        <v>100</v>
-      </c>
-      <c r="J43" t="s">
-        <v>100</v>
-      </c>
-      <c r="K43" t="s">
         <v>99</v>
-      </c>
-      <c r="L43" t="s">
-        <v>126</v>
-      </c>
-      <c r="M43" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>58</v>
-      </c>
-      <c r="B44" t="s">
-        <v>58</v>
-      </c>
-      <c r="C44" t="s">
-        <v>4</v>
-      </c>
-      <c r="D44" t="s">
-        <v>12</v>
-      </c>
-      <c r="E44" t="s">
-        <v>73</v>
-      </c>
-      <c r="F44" t="s">
-        <v>95</v>
-      </c>
-      <c r="G44" t="s">
-        <v>100</v>
-      </c>
-      <c r="H44" t="s">
-        <v>100</v>
-      </c>
-      <c r="I44" t="s">
-        <v>100</v>
-      </c>
-      <c r="J44" t="s">
-        <v>100</v>
-      </c>
-      <c r="K44" t="s">
-        <v>100</v>
-      </c>
-      <c r="L44" t="s">
-        <v>126</v>
-      </c>
-      <c r="M44" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>54</v>
-      </c>
-      <c r="B45" t="s">
-        <v>54</v>
-      </c>
-      <c r="C45" t="s">
-        <v>4</v>
-      </c>
-      <c r="D45" t="s">
-        <v>5</v>
-      </c>
-      <c r="E45" t="s">
-        <v>73</v>
-      </c>
-      <c r="F45" t="s">
-        <v>94</v>
-      </c>
-      <c r="G45" t="s">
-        <v>73</v>
-      </c>
-      <c r="H45" t="s">
-        <v>96</v>
-      </c>
-      <c r="I45" t="s">
-        <v>100</v>
-      </c>
-      <c r="J45" t="s">
-        <v>188</v>
-      </c>
-      <c r="K45" t="s">
-        <v>98</v>
-      </c>
-      <c r="L45" t="s">
-        <v>126</v>
-      </c>
-      <c r="M45" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>55</v>
-      </c>
-      <c r="B46" t="s">
-        <v>55</v>
-      </c>
-      <c r="C46" t="s">
-        <v>4</v>
-      </c>
-      <c r="D46" t="s">
-        <v>26</v>
-      </c>
-      <c r="E46" t="s">
-        <v>74</v>
-      </c>
-      <c r="F46" t="s">
-        <v>144</v>
-      </c>
-      <c r="G46" t="s">
-        <v>100</v>
-      </c>
-      <c r="H46" t="s">
-        <v>100</v>
-      </c>
-      <c r="I46" t="s">
-        <v>100</v>
-      </c>
-      <c r="J46" t="s">
-        <v>100</v>
-      </c>
-      <c r="K46" t="s">
-        <v>189</v>
-      </c>
-      <c r="L46" t="s">
-        <v>126</v>
-      </c>
-      <c r="M46" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>45</v>
-      </c>
-      <c r="B47" t="s">
-        <v>45</v>
-      </c>
-      <c r="C47" t="s">
-        <v>4</v>
-      </c>
-      <c r="D47" t="s">
-        <v>46</v>
-      </c>
-      <c r="E47" t="s">
-        <v>73</v>
-      </c>
-      <c r="F47" t="s">
-        <v>139</v>
-      </c>
-      <c r="G47" t="s">
-        <v>100</v>
-      </c>
-      <c r="H47" t="s">
-        <v>100</v>
-      </c>
-      <c r="I47" t="s">
-        <v>100</v>
-      </c>
-      <c r="J47" t="s">
-        <v>100</v>
-      </c>
-      <c r="K47" t="s">
-        <v>125</v>
-      </c>
-      <c r="L47" t="s">
-        <v>126</v>
-      </c>
-      <c r="M47" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>40</v>
-      </c>
-      <c r="B48" t="s">
-        <v>41</v>
-      </c>
-      <c r="C48" t="s">
-        <v>6</v>
-      </c>
-      <c r="D48" t="s">
-        <v>5</v>
-      </c>
-      <c r="E48" t="s">
-        <v>74</v>
-      </c>
-      <c r="F48" t="s">
-        <v>178</v>
-      </c>
-      <c r="G48" t="s">
-        <v>100</v>
-      </c>
-      <c r="H48" t="s">
-        <v>100</v>
-      </c>
-      <c r="I48" t="s">
-        <v>100</v>
-      </c>
-      <c r="J48" t="s">
-        <v>100</v>
-      </c>
-      <c r="K48" t="s">
-        <v>100</v>
-      </c>
-      <c r="L48" t="s">
-        <v>126</v>
-      </c>
-      <c r="M48" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>25</v>
-      </c>
-      <c r="B49" t="s">
-        <v>25</v>
-      </c>
-      <c r="C49" t="s">
-        <v>4</v>
-      </c>
-      <c r="D49" t="s">
-        <v>12</v>
-      </c>
-      <c r="E49" t="s">
-        <v>73</v>
-      </c>
-      <c r="F49" t="s">
-        <v>191</v>
-      </c>
-      <c r="G49" t="s">
-        <v>73</v>
-      </c>
-      <c r="H49" t="s">
-        <v>100</v>
-      </c>
-      <c r="I49" t="s">
-        <v>100</v>
-      </c>
-      <c r="J49" t="s">
-        <v>100</v>
-      </c>
-      <c r="K49" t="s">
-        <v>131</v>
-      </c>
-      <c r="L49" t="s">
-        <v>126</v>
-      </c>
-      <c r="M49" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>43</v>
-      </c>
-      <c r="B50" t="s">
-        <v>43</v>
-      </c>
-      <c r="C50" t="s">
-        <v>4</v>
-      </c>
-      <c r="D50" t="s">
-        <v>5</v>
-      </c>
-      <c r="E50" t="s">
-        <v>73</v>
-      </c>
-      <c r="F50" t="s">
-        <v>191</v>
-      </c>
-      <c r="G50" t="s">
-        <v>73</v>
-      </c>
-      <c r="H50" t="s">
-        <v>100</v>
-      </c>
-      <c r="I50" t="s">
-        <v>100</v>
-      </c>
-      <c r="J50" t="s">
-        <v>100</v>
-      </c>
-      <c r="K50" t="s">
-        <v>131</v>
-      </c>
-      <c r="L50" t="s">
-        <v>126</v>
-      </c>
-      <c r="M50" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>30</v>
-      </c>
-      <c r="B51" t="s">
-        <v>30</v>
-      </c>
-      <c r="C51" t="s">
-        <v>4</v>
-      </c>
-      <c r="D51" t="s">
-        <v>29</v>
-      </c>
-      <c r="E51" t="s">
-        <v>74</v>
-      </c>
-      <c r="F51" t="s">
-        <v>82</v>
-      </c>
-      <c r="G51" t="s">
-        <v>74</v>
-      </c>
-      <c r="H51" t="s">
-        <v>100</v>
-      </c>
-      <c r="I51" t="s">
-        <v>100</v>
-      </c>
-      <c r="J51" t="s">
-        <v>100</v>
-      </c>
-      <c r="K51" t="s">
-        <v>86</v>
-      </c>
-      <c r="L51" t="s">
-        <v>126</v>
-      </c>
-      <c r="M51" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>63</v>
-      </c>
-      <c r="B52" t="s">
-        <v>63</v>
-      </c>
-      <c r="C52" t="s">
-        <v>4</v>
-      </c>
-      <c r="D52" t="s">
-        <v>19</v>
-      </c>
-      <c r="E52" t="s">
-        <v>73</v>
-      </c>
-      <c r="F52" t="s">
-        <v>82</v>
-      </c>
-      <c r="G52" t="s">
-        <v>74</v>
-      </c>
-      <c r="H52" t="s">
-        <v>100</v>
-      </c>
-      <c r="I52" t="s">
-        <v>100</v>
-      </c>
-      <c r="J52" t="s">
-        <v>100</v>
-      </c>
-      <c r="K52" t="s">
-        <v>86</v>
-      </c>
-      <c r="L52" t="s">
-        <v>126</v>
-      </c>
-      <c r="M52" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>67</v>
-      </c>
-      <c r="B53" t="s">
-        <v>67</v>
-      </c>
-      <c r="C53" t="s">
-        <v>4</v>
-      </c>
-      <c r="D53" t="s">
-        <v>36</v>
-      </c>
-      <c r="E53" t="s">
-        <v>73</v>
-      </c>
-      <c r="F53" t="s">
-        <v>82</v>
-      </c>
-      <c r="G53" t="s">
-        <v>74</v>
-      </c>
-      <c r="H53" t="s">
-        <v>100</v>
-      </c>
-      <c r="I53" t="s">
-        <v>100</v>
-      </c>
-      <c r="J53" t="s">
-        <v>100</v>
-      </c>
-      <c r="K53" t="s">
-        <v>100</v>
-      </c>
-      <c r="L53" t="s">
-        <v>126</v>
-      </c>
-      <c r="M53" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>48</v>
-      </c>
-      <c r="B54" t="s">
-        <v>48</v>
-      </c>
-      <c r="C54" t="s">
-        <v>4</v>
-      </c>
-      <c r="D54" t="s">
-        <v>19</v>
-      </c>
-      <c r="E54" t="s">
-        <v>73</v>
-      </c>
-      <c r="F54" t="s">
-        <v>83</v>
-      </c>
-      <c r="G54" t="s">
-        <v>73</v>
-      </c>
-      <c r="H54" t="s">
-        <v>100</v>
-      </c>
-      <c r="I54" t="s">
-        <v>100</v>
-      </c>
-      <c r="J54" t="s">
-        <v>100</v>
-      </c>
-      <c r="K54" t="s">
-        <v>100</v>
-      </c>
-      <c r="L54" t="s">
-        <v>126</v>
-      </c>
-      <c r="M54" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>67</v>
-      </c>
-      <c r="B55" t="s">
-        <v>67</v>
-      </c>
-      <c r="C55" t="s">
-        <v>4</v>
-      </c>
-      <c r="D55" t="s">
-        <v>36</v>
-      </c>
-      <c r="E55" t="s">
-        <v>73</v>
-      </c>
-      <c r="F55" t="s">
-        <v>83</v>
-      </c>
-      <c r="G55" t="s">
-        <v>73</v>
-      </c>
-      <c r="H55" t="s">
-        <v>100</v>
-      </c>
-      <c r="I55" t="s">
-        <v>100</v>
-      </c>
-      <c r="J55" t="s">
-        <v>100</v>
-      </c>
-      <c r="K55" t="s">
-        <v>100</v>
-      </c>
-      <c r="L55" t="s">
-        <v>126</v>
-      </c>
-      <c r="M55" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>24</v>
-      </c>
-      <c r="B56" t="s">
-        <v>24</v>
-      </c>
-      <c r="C56" t="s">
-        <v>4</v>
-      </c>
-      <c r="D56" t="s">
-        <v>12</v>
-      </c>
-      <c r="E56" t="s">
-        <v>74</v>
-      </c>
-      <c r="F56" t="s">
-        <v>119</v>
-      </c>
-      <c r="G56" t="s">
-        <v>74</v>
-      </c>
-      <c r="H56" t="s">
-        <v>100</v>
-      </c>
-      <c r="I56" t="s">
-        <v>100</v>
-      </c>
-      <c r="J56" t="s">
-        <v>100</v>
-      </c>
-      <c r="K56" t="s">
-        <v>120</v>
-      </c>
-      <c r="L56" t="s">
-        <v>126</v>
-      </c>
-      <c r="M56" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>66</v>
-      </c>
-      <c r="B57" t="s">
-        <v>66</v>
-      </c>
-      <c r="C57" t="s">
-        <v>4</v>
-      </c>
-      <c r="D57" t="s">
-        <v>27</v>
-      </c>
-      <c r="E57" t="s">
-        <v>73</v>
-      </c>
-      <c r="F57" t="s">
-        <v>149</v>
-      </c>
-      <c r="G57" t="s">
-        <v>73</v>
-      </c>
-      <c r="H57" t="s">
-        <v>190</v>
-      </c>
-      <c r="I57" t="s">
-        <v>100</v>
-      </c>
-      <c r="J57" t="s">
-        <v>100</v>
-      </c>
-      <c r="K57" t="s">
-        <v>100</v>
-      </c>
-      <c r="L57" t="s">
-        <v>126</v>
-      </c>
-      <c r="M57" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>13</v>
-      </c>
-      <c r="B58" t="s">
-        <v>13</v>
-      </c>
-      <c r="C58" t="s">
-        <v>4</v>
-      </c>
-      <c r="D58" t="s">
-        <v>5</v>
-      </c>
-      <c r="E58" t="s">
-        <v>73</v>
-      </c>
-      <c r="F58" t="s">
-        <v>184</v>
-      </c>
-      <c r="G58" t="s">
-        <v>73</v>
-      </c>
-      <c r="H58" t="s">
-        <v>225</v>
-      </c>
-      <c r="I58" t="s">
-        <v>100</v>
-      </c>
-      <c r="J58" t="s">
-        <v>5</v>
-      </c>
-      <c r="K58" t="s">
-        <v>84</v>
-      </c>
-      <c r="L58" t="s">
-        <v>126</v>
-      </c>
-      <c r="M58" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>37</v>
-      </c>
-      <c r="B59" t="s">
-        <v>37</v>
-      </c>
-      <c r="C59" t="s">
-        <v>4</v>
-      </c>
-      <c r="D59" t="s">
-        <v>36</v>
-      </c>
-      <c r="E59" t="s">
-        <v>73</v>
-      </c>
-      <c r="F59" t="s">
-        <v>184</v>
-      </c>
-      <c r="G59" t="s">
-        <v>73</v>
-      </c>
-      <c r="H59" t="s">
-        <v>116</v>
-      </c>
-      <c r="I59" t="s">
-        <v>100</v>
-      </c>
-      <c r="J59" t="s">
-        <v>117</v>
-      </c>
-      <c r="K59" t="s">
-        <v>84</v>
-      </c>
-      <c r="L59" t="s">
-        <v>126</v>
-      </c>
-      <c r="M59" t="s">
-        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
even more consolidation and cleanup
</commit_message>
<xml_diff>
--- a/argot/working_docs/endeca_fields_to_Argot.xlsx
+++ b/argot/working_docs/endeca_fields_to_Argot.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="106">
   <si>
     <t>Element name</t>
   </si>
@@ -49,57 +49,18 @@
     <t>Keyword</t>
   </si>
   <si>
-    <t>Collective Uniform Title</t>
-  </si>
-  <si>
     <t>Author, Author_Brief, Keyword, Keyword_Brief</t>
   </si>
   <si>
-    <t>Keyword, Keyword_Brief, Title</t>
-  </si>
-  <si>
     <t>Format</t>
   </si>
   <si>
-    <t>ICE Chapter Title</t>
-  </si>
-  <si>
-    <t>Indexed Notes</t>
-  </si>
-  <si>
-    <t>ISBN</t>
-  </si>
-  <si>
-    <t>ISBN, Keyword</t>
-  </si>
-  <si>
-    <t>Journal_Concise, Journal_Title</t>
-  </si>
-  <si>
-    <t>Journal Title Abbreviation</t>
-  </si>
-  <si>
     <t>LocalId</t>
   </si>
   <si>
-    <t>Main Series Linking</t>
-  </si>
-  <si>
-    <t>Keyword, Keyword_Brief, Title, Title_Brief</t>
-  </si>
-  <si>
-    <t>Main Uniform Title</t>
-  </si>
-  <si>
     <t>Material Details</t>
   </si>
   <si>
-    <t>Medical Subject</t>
-  </si>
-  <si>
-    <t>Medical Subject: Topic</t>
-  </si>
-  <si>
     <t>Musical Presentation</t>
   </si>
   <si>
@@ -109,15 +70,6 @@
     <t>Organization</t>
   </si>
   <si>
-    <t>Other Author Translation</t>
-  </si>
-  <si>
-    <t>Author, Keyword, Keyword_Brief</t>
-  </si>
-  <si>
-    <t>Other Title Translation</t>
-  </si>
-  <si>
     <t>Performer Credits</t>
   </si>
   <si>
@@ -127,33 +79,12 @@
     <t>PubDateSort</t>
   </si>
   <si>
-    <t>Series</t>
-  </si>
-  <si>
-    <t>Series ISSN</t>
-  </si>
-  <si>
-    <t>Series Statement</t>
-  </si>
-  <si>
-    <t>Subseries Linking</t>
-  </si>
-  <si>
     <t>Syndetics ISBN</t>
   </si>
   <si>
     <t>Syndetics_ISBN</t>
   </si>
   <si>
-    <t>Title Index</t>
-  </si>
-  <si>
-    <t>UPC</t>
-  </si>
-  <si>
-    <t>Varying Titles</t>
-  </si>
-  <si>
     <t>Displayed Endeca?</t>
   </si>
   <si>
@@ -175,18 +106,6 @@
     <t>Label</t>
   </si>
   <si>
-    <t>title_variant_access</t>
-  </si>
-  <si>
-    <t>title_variant_note</t>
-  </si>
-  <si>
-    <t>Title portion indexed in indexed-only title_uniform.  Author portion indexed in author_main. Stored for display and creation of hyperlink</t>
-  </si>
-  <si>
-    <t>These are indexed only titles, including variants coded as index-only in 246, abbreviated title</t>
-  </si>
-  <si>
     <t>resource_type</t>
   </si>
   <si>
@@ -196,24 +115,6 @@
     <t>Facet values, but should also probably display on each record</t>
   </si>
   <si>
-    <t>series_transcribed</t>
-  </si>
-  <si>
-    <t>series_collocation</t>
-  </si>
-  <si>
-    <t>Details &gt; Series</t>
-  </si>
-  <si>
-    <t>Related works &gt; Other items in series</t>
-  </si>
-  <si>
-    <t>Includes volume designations</t>
-  </si>
-  <si>
-    <t>Hyperlinked to series query for the title -- no volume designation</t>
-  </si>
-  <si>
     <t>.</t>
   </si>
   <si>
@@ -223,21 +124,6 @@
     <t>indexed</t>
   </si>
   <si>
-    <t>Related works &gt; Other versions of this work</t>
-  </si>
-  <si>
-    <t>title; author; keyword</t>
-  </si>
-  <si>
-    <t>titles_included_ice</t>
-  </si>
-  <si>
-    <t>Display is provided by Syndetics API at load time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mapped from 242c in Endeca. Used in 2 bib records at UNC. How much do we care about this? </t>
-  </si>
-  <si>
     <t>map</t>
   </si>
   <si>
@@ -253,9 +139,6 @@
     <t>defer for EAD</t>
   </si>
   <si>
-    <t>split up into other fields</t>
-  </si>
-  <si>
     <t>check/test</t>
   </si>
   <si>
@@ -271,9 +154,6 @@
     <t>organization_and_arrangement</t>
   </si>
   <si>
-    <t>statement_of_responsibility[translation]</t>
-  </si>
-  <si>
     <t>performer_credits</t>
   </si>
   <si>
@@ -286,9 +166,6 @@
     <t>(in Endeca, drives Publication Year facet)</t>
   </si>
   <si>
-    <t>series_transcribed[issn]; series_collocation[issn]</t>
-  </si>
-  <si>
     <t>defer for shared records</t>
   </si>
   <si>
@@ -298,30 +175,15 @@
     <t>example: https://ingest.discovery.trln.org/record/search?id=UNCb2398669</t>
   </si>
   <si>
-    <t>upc</t>
-  </si>
-  <si>
     <t>ticket</t>
   </si>
   <si>
     <t>https://trlnmain.atlassian.net/browse/TD-462</t>
   </si>
   <si>
-    <t>https://trlnmain.atlassian.net/browse/TD-442</t>
-  </si>
-  <si>
     <t>https://trlnmain.atlassian.net/browse/TD-434</t>
   </si>
   <si>
-    <t>https://trlnmain.atlassian.net/browse/TD-464</t>
-  </si>
-  <si>
-    <t>https://trlnmain.atlassian.net/browse/TD-465</t>
-  </si>
-  <si>
-    <t>https://trlnmain.atlassian.net/browse/TD-392</t>
-  </si>
-  <si>
     <t>https://trlnmain.atlassian.net/browse/TD-466</t>
   </si>
   <si>
@@ -331,15 +193,6 @@
     <t>https://trlnmain.atlassian.net/browse/TD-435</t>
   </si>
   <si>
-    <t>https://trlnmain.atlassian.net/browse/TD-160</t>
-  </si>
-  <si>
-    <t>https://trlnmain.atlassian.net/browse/TD-475</t>
-  </si>
-  <si>
-    <t>https://trlnmain.atlassian.net/browse/TD-331</t>
-  </si>
-  <si>
     <t>https://trlnmain.atlassian.net/browse/TD-477</t>
   </si>
   <si>
@@ -370,12 +223,6 @@
     <t>https://trlnmain.atlassian.net/browse/TD-482</t>
   </si>
   <si>
-    <t>subject_heading_mesh</t>
-  </si>
-  <si>
-    <t>https://trlnmain.atlassian.net/browse/TD-131</t>
-  </si>
-  <si>
     <t>document - done in spreadsheet.</t>
   </si>
   <si>
@@ -385,24 +232,6 @@
     <t>Decision needed</t>
   </si>
   <si>
-    <t>work_name_title</t>
-  </si>
-  <si>
-    <t>https://trlnmain.atlassian.net/browse/TD-493</t>
-  </si>
-  <si>
-    <t>series; title; keyword</t>
-  </si>
-  <si>
-    <t>Displayed as part of the series value shown, but not part of series_collocation link.</t>
-  </si>
-  <si>
-    <t>IDs &gt; UPC</t>
-  </si>
-  <si>
-    <t>tbd</t>
-  </si>
-  <si>
     <t>Column(s)</t>
   </si>
   <si>
@@ -491,9 +320,6 @@
   </si>
   <si>
     <t xml:space="preserve">This is based on the set of all Endeca property and dimensions that were not already mapped into Argot when I began this work. </t>
-  </si>
-  <si>
-    <t>Related items &gt; ??</t>
   </si>
   <si>
     <t>Display notes</t>
@@ -1126,8 +952,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="endecafields" displayName="endecafields" ref="A1:M33" totalsRowShown="0">
-  <autoFilter ref="A1:M33"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="endecafields" displayName="endecafields" ref="A1:M15" totalsRowShown="0">
+  <autoFilter ref="A1:M15"/>
   <tableColumns count="13">
     <tableColumn id="1" name="Element name"/>
     <tableColumn id="2" name="Endeca dmod name"/>
@@ -1424,16 +1250,16 @@
   <sheetData>
     <row r="1" spans="1:2" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>156</v>
+        <v>99</v>
       </c>
       <c r="B1" s="2"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>127</v>
+        <v>70</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>128</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -1441,7 +1267,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>129</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -1449,7 +1275,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>130</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1457,7 +1283,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>131</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1465,175 +1291,175 @@
         <v>3</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>132</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>133</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>134</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>135</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>136</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>66</v>
+        <v>33</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>137</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>139</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>138</v>
+        <v>81</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>140</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>93</v>
+        <v>51</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>141</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>142</v>
+        <v>85</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>143</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>78</v>
+        <v>39</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>144</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>120</v>
+        <v>69</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>145</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>74</v>
+        <v>36</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>146</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>76</v>
+        <v>38</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>147</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>79</v>
+        <v>40</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>148</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>89</v>
+        <v>48</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>149</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>75</v>
+        <v>37</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>151</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>118</v>
+        <v>67</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>150</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>73</v>
+        <v>35</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>152</v>
+        <v>95</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>72</v>
+        <v>34</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>153</v>
+        <v>96</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>154</v>
+        <v>97</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>119</v>
+        <v>68</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>155</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1650,10 +1476,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M33"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD16"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1680,39 +1506,39 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="F1" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="G1" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="H1" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="I1" t="s">
-        <v>158</v>
+        <v>100</v>
       </c>
       <c r="J1" t="s">
-        <v>66</v>
+        <v>33</v>
       </c>
       <c r="K1" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="L1" t="s">
-        <v>138</v>
+        <v>81</v>
       </c>
       <c r="M1" t="s">
-        <v>93</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -1721,39 +1547,39 @@
         <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="F2" t="s">
-        <v>80</v>
+        <v>41</v>
       </c>
       <c r="G2" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="H2" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="I2" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="J2" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="K2" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="L2" t="s">
-        <v>75</v>
+        <v>37</v>
       </c>
       <c r="M2" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -1762,39 +1588,39 @@
         <v>5</v>
       </c>
       <c r="E3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" t="s">
+        <v>31</v>
+      </c>
+      <c r="K3" t="s">
         <v>47</v>
       </c>
-      <c r="F3" t="s">
-        <v>86</v>
-      </c>
-      <c r="G3" t="s">
-        <v>64</v>
-      </c>
-      <c r="H3" t="s">
-        <v>64</v>
-      </c>
-      <c r="I3" t="s">
-        <v>64</v>
-      </c>
-      <c r="J3" t="s">
-        <v>64</v>
-      </c>
-      <c r="K3" t="s">
-        <v>87</v>
-      </c>
       <c r="L3" t="s">
-        <v>75</v>
+        <v>37</v>
       </c>
       <c r="M3" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -1803,31 +1629,31 @@
         <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="F4" t="s">
-        <v>90</v>
+        <v>49</v>
       </c>
       <c r="G4" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="H4" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="I4" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="J4" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="K4" t="s">
-        <v>91</v>
+        <v>50</v>
       </c>
       <c r="L4" t="s">
-        <v>75</v>
+        <v>37</v>
       </c>
       <c r="M4" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -1844,39 +1670,39 @@
         <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="F5" t="s">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="G5" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="H5" t="s">
-        <v>163</v>
+        <v>105</v>
       </c>
       <c r="I5" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="J5" t="s">
         <v>5</v>
       </c>
       <c r="K5" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="L5" t="s">
-        <v>72</v>
+        <v>34</v>
       </c>
       <c r="M5" t="s">
-        <v>94</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -1885,39 +1711,39 @@
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="F6" t="s">
-        <v>111</v>
+        <v>62</v>
       </c>
       <c r="G6" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="H6" t="s">
-        <v>162</v>
+        <v>104</v>
       </c>
       <c r="I6" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="J6" t="s">
         <v>5</v>
       </c>
       <c r="K6" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="L6" t="s">
-        <v>72</v>
+        <v>34</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>115</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -1926,39 +1752,39 @@
         <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="F7" t="s">
-        <v>109</v>
+        <v>60</v>
       </c>
       <c r="G7" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="H7" t="s">
-        <v>161</v>
+        <v>103</v>
       </c>
       <c r="I7" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="J7" t="s">
         <v>5</v>
       </c>
       <c r="K7" t="s">
+        <v>31</v>
+      </c>
+      <c r="L7" t="s">
+        <v>34</v>
+      </c>
+      <c r="M7" t="s">
         <v>64</v>
-      </c>
-      <c r="L7" t="s">
-        <v>72</v>
-      </c>
-      <c r="M7" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -1967,39 +1793,39 @@
         <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="F8" t="s">
-        <v>108</v>
+        <v>59</v>
       </c>
       <c r="G8" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="H8" t="s">
-        <v>160</v>
+        <v>102</v>
       </c>
       <c r="I8" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="J8" t="s">
         <v>5</v>
       </c>
       <c r="K8" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="L8" t="s">
-        <v>72</v>
+        <v>34</v>
       </c>
       <c r="M8" t="s">
-        <v>112</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -2008,39 +1834,39 @@
         <v>5</v>
       </c>
       <c r="E9" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="F9" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="G9" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="H9" t="s">
-        <v>159</v>
+        <v>101</v>
       </c>
       <c r="I9" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="J9" t="s">
         <v>5</v>
       </c>
       <c r="K9" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="L9" t="s">
-        <v>72</v>
+        <v>34</v>
       </c>
       <c r="M9" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -2049,39 +1875,39 @@
         <v>5</v>
       </c>
       <c r="E10" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="F10" t="s">
-        <v>81</v>
+        <v>42</v>
       </c>
       <c r="G10" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="H10" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="I10" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="J10" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="K10" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="L10" t="s">
-        <v>72</v>
+        <v>34</v>
       </c>
       <c r="M10" t="s">
-        <v>107</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -2090,80 +1916,80 @@
         <v>5</v>
       </c>
       <c r="E11" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="F11" t="s">
-        <v>82</v>
+        <v>43</v>
       </c>
       <c r="G11" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="H11" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="I11" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="J11" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="K11" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="L11" t="s">
-        <v>72</v>
+        <v>34</v>
       </c>
       <c r="M11" t="s">
-        <v>106</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E12" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="F12" t="s">
-        <v>84</v>
+        <v>44</v>
       </c>
       <c r="G12" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="H12" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="I12" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="J12" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="K12" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="L12" t="s">
-        <v>72</v>
+        <v>34</v>
       </c>
       <c r="M12" t="s">
-        <v>100</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C13" t="s">
         <v>6</v>
@@ -2172,80 +1998,80 @@
         <v>5</v>
       </c>
       <c r="E13" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="F13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I13" t="s">
+        <v>31</v>
+      </c>
+      <c r="J13" t="s">
+        <v>31</v>
+      </c>
+      <c r="K13" t="s">
+        <v>30</v>
+      </c>
+      <c r="L13" t="s">
+        <v>34</v>
+      </c>
+      <c r="M13" t="s">
         <v>56</v>
-      </c>
-      <c r="G13" t="s">
-        <v>47</v>
-      </c>
-      <c r="H13" t="s">
-        <v>64</v>
-      </c>
-      <c r="I13" t="s">
-        <v>64</v>
-      </c>
-      <c r="J13" t="s">
-        <v>64</v>
-      </c>
-      <c r="K13" t="s">
-        <v>57</v>
-      </c>
-      <c r="L13" t="s">
-        <v>72</v>
-      </c>
-      <c r="M13" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E14" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="F14" t="s">
-        <v>85</v>
+        <v>45</v>
       </c>
       <c r="G14" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="H14" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="I14" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="J14" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="K14" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="L14" t="s">
-        <v>72</v>
+        <v>34</v>
       </c>
       <c r="M14" t="s">
-        <v>101</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C15" t="s">
         <v>6</v>
@@ -2254,769 +2080,31 @@
         <v>5</v>
       </c>
       <c r="E15" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="F15" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="G15" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="H15" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="I15" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="J15" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="K15" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="L15" t="s">
-        <v>72</v>
+        <v>34</v>
       </c>
       <c r="M15" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" t="s">
-        <v>5</v>
-      </c>
-      <c r="E16" t="s">
-        <v>47</v>
-      </c>
-      <c r="F16" t="s">
-        <v>59</v>
-      </c>
-      <c r="G16" t="s">
-        <v>64</v>
-      </c>
-      <c r="H16" t="s">
-        <v>64</v>
-      </c>
-      <c r="I16" t="s">
-        <v>64</v>
-      </c>
-      <c r="J16" t="s">
-        <v>64</v>
-      </c>
-      <c r="K16" t="s">
-        <v>64</v>
-      </c>
-      <c r="L16" t="s">
-        <v>72</v>
-      </c>
-      <c r="M16" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" t="s">
-        <v>47</v>
-      </c>
-      <c r="F17" t="s">
-        <v>59</v>
-      </c>
-      <c r="G17" t="s">
-        <v>47</v>
-      </c>
-      <c r="H17" t="s">
-        <v>61</v>
-      </c>
-      <c r="I17" t="s">
-        <v>64</v>
-      </c>
-      <c r="J17" t="s">
-        <v>64</v>
-      </c>
-      <c r="K17" t="s">
-        <v>63</v>
-      </c>
-      <c r="L17" t="s">
-        <v>72</v>
-      </c>
-      <c r="M17" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" t="s">
-        <v>47</v>
-      </c>
-      <c r="F18" t="s">
-        <v>59</v>
-      </c>
-      <c r="G18" t="s">
-        <v>64</v>
-      </c>
-      <c r="H18" t="s">
-        <v>64</v>
-      </c>
-      <c r="I18" t="s">
-        <v>64</v>
-      </c>
-      <c r="J18" t="s">
-        <v>64</v>
-      </c>
-      <c r="K18" t="s">
-        <v>64</v>
-      </c>
-      <c r="L18" t="s">
-        <v>72</v>
-      </c>
-      <c r="M18" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" t="s">
-        <v>35</v>
-      </c>
-      <c r="C19" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" t="s">
-        <v>5</v>
-      </c>
-      <c r="E19" t="s">
-        <v>47</v>
-      </c>
-      <c r="F19" t="s">
-        <v>58</v>
-      </c>
-      <c r="G19" t="s">
-        <v>47</v>
-      </c>
-      <c r="H19" t="s">
-        <v>60</v>
-      </c>
-      <c r="I19" t="s">
-        <v>64</v>
-      </c>
-      <c r="J19" t="s">
-        <v>123</v>
-      </c>
-      <c r="K19" t="s">
-        <v>62</v>
-      </c>
-      <c r="L19" t="s">
-        <v>72</v>
-      </c>
-      <c r="M19" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" t="s">
-        <v>36</v>
-      </c>
-      <c r="C20" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" t="s">
-        <v>15</v>
-      </c>
-      <c r="E20" t="s">
-        <v>48</v>
-      </c>
-      <c r="F20" t="s">
-        <v>88</v>
-      </c>
-      <c r="G20" t="s">
-        <v>64</v>
-      </c>
-      <c r="H20" t="s">
-        <v>64</v>
-      </c>
-      <c r="I20" t="s">
-        <v>64</v>
-      </c>
-      <c r="J20" t="s">
-        <v>64</v>
-      </c>
-      <c r="K20" t="s">
-        <v>124</v>
-      </c>
-      <c r="L20" t="s">
-        <v>72</v>
-      </c>
-      <c r="M20" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>29</v>
-      </c>
-      <c r="B21" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" t="s">
-        <v>30</v>
-      </c>
-      <c r="E21" t="s">
-        <v>47</v>
-      </c>
-      <c r="F21" t="s">
-        <v>83</v>
-      </c>
-      <c r="G21" t="s">
-        <v>64</v>
-      </c>
-      <c r="H21" t="s">
-        <v>64</v>
-      </c>
-      <c r="I21" t="s">
-        <v>64</v>
-      </c>
-      <c r="J21" t="s">
-        <v>64</v>
-      </c>
-      <c r="K21" t="s">
-        <v>71</v>
-      </c>
-      <c r="L21" t="s">
-        <v>72</v>
-      </c>
-      <c r="M21" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>24</v>
-      </c>
-      <c r="B22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C22" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" t="s">
-        <v>5</v>
-      </c>
-      <c r="E22" t="s">
-        <v>48</v>
-      </c>
-      <c r="F22" t="s">
-        <v>116</v>
-      </c>
-      <c r="G22" t="s">
-        <v>64</v>
-      </c>
-      <c r="H22" t="s">
-        <v>64</v>
-      </c>
-      <c r="I22" t="s">
-        <v>64</v>
-      </c>
-      <c r="J22" t="s">
-        <v>64</v>
-      </c>
-      <c r="K22" t="s">
-        <v>64</v>
-      </c>
-      <c r="L22" t="s">
-        <v>72</v>
-      </c>
-      <c r="M22" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>14</v>
-      </c>
-      <c r="B23" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" t="s">
-        <v>8</v>
-      </c>
-      <c r="E23" t="s">
-        <v>47</v>
-      </c>
-      <c r="F23" t="s">
-        <v>126</v>
-      </c>
-      <c r="G23" t="s">
-        <v>47</v>
-      </c>
-      <c r="H23" t="s">
-        <v>64</v>
-      </c>
-      <c r="I23" t="s">
-        <v>64</v>
-      </c>
-      <c r="J23" t="s">
-        <v>64</v>
-      </c>
-      <c r="K23" t="s">
-        <v>77</v>
-      </c>
-      <c r="L23" t="s">
-        <v>72</v>
-      </c>
-      <c r="M23" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24" t="s">
-        <v>5</v>
-      </c>
-      <c r="E24" t="s">
-        <v>47</v>
-      </c>
-      <c r="F24" t="s">
-        <v>126</v>
-      </c>
-      <c r="G24" t="s">
-        <v>47</v>
-      </c>
-      <c r="H24" t="s">
-        <v>64</v>
-      </c>
-      <c r="I24" t="s">
-        <v>64</v>
-      </c>
-      <c r="J24" t="s">
-        <v>64</v>
-      </c>
-      <c r="K24" t="s">
-        <v>77</v>
-      </c>
-      <c r="L24" t="s">
-        <v>72</v>
-      </c>
-      <c r="M24" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>18</v>
-      </c>
-      <c r="B25" t="s">
-        <v>18</v>
-      </c>
-      <c r="C25" t="s">
-        <v>4</v>
-      </c>
-      <c r="D25" t="s">
-        <v>17</v>
-      </c>
-      <c r="E25" t="s">
-        <v>48</v>
-      </c>
-      <c r="F25" t="s">
-        <v>51</v>
-      </c>
-      <c r="G25" t="s">
-        <v>48</v>
-      </c>
-      <c r="H25" t="s">
-        <v>64</v>
-      </c>
-      <c r="I25" t="s">
-        <v>64</v>
-      </c>
-      <c r="J25" t="s">
-        <v>64</v>
-      </c>
-      <c r="K25" t="s">
-        <v>54</v>
-      </c>
-      <c r="L25" t="s">
-        <v>72</v>
-      </c>
-      <c r="M25" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>41</v>
-      </c>
-      <c r="B26" t="s">
-        <v>41</v>
-      </c>
-      <c r="C26" t="s">
-        <v>4</v>
-      </c>
-      <c r="D26" t="s">
-        <v>11</v>
-      </c>
-      <c r="E26" t="s">
-        <v>47</v>
-      </c>
-      <c r="F26" t="s">
-        <v>51</v>
-      </c>
-      <c r="G26" t="s">
-        <v>48</v>
-      </c>
-      <c r="H26" t="s">
-        <v>64</v>
-      </c>
-      <c r="I26" t="s">
-        <v>64</v>
-      </c>
-      <c r="J26" t="s">
-        <v>64</v>
-      </c>
-      <c r="K26" t="s">
-        <v>54</v>
-      </c>
-      <c r="L26" t="s">
-        <v>72</v>
-      </c>
-      <c r="M26" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>43</v>
-      </c>
-      <c r="B27" t="s">
-        <v>43</v>
-      </c>
-      <c r="C27" t="s">
-        <v>4</v>
-      </c>
-      <c r="D27" t="s">
-        <v>21</v>
-      </c>
-      <c r="E27" t="s">
-        <v>47</v>
-      </c>
-      <c r="F27" t="s">
-        <v>51</v>
-      </c>
-      <c r="G27" t="s">
-        <v>48</v>
-      </c>
-      <c r="H27" t="s">
-        <v>64</v>
-      </c>
-      <c r="I27" t="s">
-        <v>64</v>
-      </c>
-      <c r="J27" t="s">
-        <v>64</v>
-      </c>
-      <c r="K27" t="s">
-        <v>64</v>
-      </c>
-      <c r="L27" t="s">
-        <v>72</v>
-      </c>
-      <c r="M27" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B28" t="s">
-        <v>31</v>
-      </c>
-      <c r="C28" t="s">
-        <v>4</v>
-      </c>
-      <c r="D28" t="s">
-        <v>11</v>
-      </c>
-      <c r="E28" t="s">
-        <v>47</v>
-      </c>
-      <c r="F28" t="s">
-        <v>52</v>
-      </c>
-      <c r="G28" t="s">
-        <v>47</v>
-      </c>
-      <c r="H28" t="s">
-        <v>64</v>
-      </c>
-      <c r="I28" t="s">
-        <v>64</v>
-      </c>
-      <c r="J28" t="s">
-        <v>64</v>
-      </c>
-      <c r="K28" t="s">
-        <v>64</v>
-      </c>
-      <c r="L28" t="s">
-        <v>72</v>
-      </c>
-      <c r="M28" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>43</v>
-      </c>
-      <c r="B29" t="s">
-        <v>43</v>
-      </c>
-      <c r="C29" t="s">
-        <v>4</v>
-      </c>
-      <c r="D29" t="s">
-        <v>21</v>
-      </c>
-      <c r="E29" t="s">
-        <v>47</v>
-      </c>
-      <c r="F29" t="s">
-        <v>52</v>
-      </c>
-      <c r="G29" t="s">
-        <v>47</v>
-      </c>
-      <c r="H29" t="s">
-        <v>64</v>
-      </c>
-      <c r="I29" t="s">
-        <v>64</v>
-      </c>
-      <c r="J29" t="s">
-        <v>64</v>
-      </c>
-      <c r="K29" t="s">
-        <v>64</v>
-      </c>
-      <c r="L29" t="s">
-        <v>72</v>
-      </c>
-      <c r="M29" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>13</v>
-      </c>
-      <c r="B30" t="s">
-        <v>13</v>
-      </c>
-      <c r="C30" t="s">
-        <v>4</v>
-      </c>
-      <c r="D30" t="s">
-        <v>8</v>
-      </c>
-      <c r="E30" t="s">
-        <v>48</v>
-      </c>
-      <c r="F30" t="s">
-        <v>69</v>
-      </c>
-      <c r="G30" t="s">
-        <v>48</v>
-      </c>
-      <c r="H30" t="s">
-        <v>64</v>
-      </c>
-      <c r="I30" t="s">
-        <v>64</v>
-      </c>
-      <c r="J30" t="s">
-        <v>64</v>
-      </c>
-      <c r="K30" t="s">
-        <v>70</v>
-      </c>
-      <c r="L30" t="s">
-        <v>72</v>
-      </c>
-      <c r="M30" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>42</v>
-      </c>
-      <c r="B31" t="s">
-        <v>42</v>
-      </c>
-      <c r="C31" t="s">
-        <v>4</v>
-      </c>
-      <c r="D31" t="s">
-        <v>16</v>
-      </c>
-      <c r="E31" t="s">
-        <v>47</v>
-      </c>
-      <c r="F31" t="s">
-        <v>92</v>
-      </c>
-      <c r="G31" t="s">
-        <v>47</v>
-      </c>
-      <c r="H31" t="s">
-        <v>125</v>
-      </c>
-      <c r="I31" t="s">
-        <v>64</v>
-      </c>
-      <c r="J31" t="s">
-        <v>64</v>
-      </c>
-      <c r="K31" t="s">
-        <v>64</v>
-      </c>
-      <c r="L31" t="s">
-        <v>72</v>
-      </c>
-      <c r="M31" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>9</v>
-      </c>
-      <c r="B32" t="s">
-        <v>9</v>
-      </c>
-      <c r="C32" t="s">
-        <v>4</v>
-      </c>
-      <c r="D32" t="s">
-        <v>5</v>
-      </c>
-      <c r="E32" t="s">
-        <v>47</v>
-      </c>
-      <c r="F32" t="s">
-        <v>121</v>
-      </c>
-      <c r="G32" t="s">
-        <v>47</v>
-      </c>
-      <c r="H32" t="s">
-        <v>157</v>
-      </c>
-      <c r="I32" t="s">
-        <v>64</v>
-      </c>
-      <c r="J32" t="s">
-        <v>5</v>
-      </c>
-      <c r="K32" t="s">
         <v>53</v>
-      </c>
-      <c r="L32" t="s">
-        <v>72</v>
-      </c>
-      <c r="M32" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>22</v>
-      </c>
-      <c r="B33" t="s">
-        <v>22</v>
-      </c>
-      <c r="C33" t="s">
-        <v>4</v>
-      </c>
-      <c r="D33" t="s">
-        <v>21</v>
-      </c>
-      <c r="E33" t="s">
-        <v>47</v>
-      </c>
-      <c r="F33" t="s">
-        <v>121</v>
-      </c>
-      <c r="G33" t="s">
-        <v>47</v>
-      </c>
-      <c r="H33" t="s">
-        <v>67</v>
-      </c>
-      <c r="I33" t="s">
-        <v>64</v>
-      </c>
-      <c r="J33" t="s">
-        <v>68</v>
-      </c>
-      <c r="K33" t="s">
-        <v>53</v>
-      </c>
-      <c r="L33" t="s">
-        <v>72</v>
-      </c>
-      <c r="M33" t="s">
-        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
note_scale and credits notes
</commit_message>
<xml_diff>
--- a/argot/working_docs/endeca_fields_to_Argot.xlsx
+++ b/argot/working_docs/endeca_fields_to_Argot.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="99">
   <si>
     <t>Element name</t>
   </si>
@@ -49,9 +49,6 @@
     <t>Keyword</t>
   </si>
   <si>
-    <t>Author, Author_Brief, Keyword, Keyword_Brief</t>
-  </si>
-  <si>
     <t>Format</t>
   </si>
   <si>
@@ -70,12 +67,6 @@
     <t>Organization</t>
   </si>
   <si>
-    <t>Performer Credits</t>
-  </si>
-  <si>
-    <t>Production Credits</t>
-  </si>
-  <si>
     <t>PubDateSort</t>
   </si>
   <si>
@@ -154,12 +145,6 @@
     <t>organization_and_arrangement</t>
   </si>
   <si>
-    <t>performer_credits</t>
-  </si>
-  <si>
-    <t>production_credits</t>
-  </si>
-  <si>
     <t>publication_year</t>
   </si>
   <si>
@@ -182,12 +167,6 @@
   </si>
   <si>
     <t>https://trlnmain.atlassian.net/browse/TD-434</t>
-  </si>
-  <si>
-    <t>https://trlnmain.atlassian.net/browse/TD-466</t>
-  </si>
-  <si>
-    <t>https://trlnmain.atlassian.net/browse/TD-467</t>
   </si>
   <si>
     <t>https://trlnmain.atlassian.net/browse/TD-435</t>
@@ -952,8 +931,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="endecafields" displayName="endecafields" ref="A1:M15" totalsRowShown="0">
-  <autoFilter ref="A1:M15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="endecafields" displayName="endecafields" ref="A1:M13" totalsRowShown="0">
+  <autoFilter ref="A1:M13"/>
   <tableColumns count="13">
     <tableColumn id="1" name="Element name"/>
     <tableColumn id="2" name="Endeca dmod name"/>
@@ -1250,16 +1229,16 @@
   <sheetData>
     <row r="1" spans="1:2" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B1" s="6"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -1267,7 +1246,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -1275,7 +1254,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1283,7 +1262,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1291,175 +1270,175 @@
         <v>3</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1476,10 +1455,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M15"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1506,39 +1485,39 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="I1" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="J1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="K1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L1" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="M1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -1547,39 +1526,39 @@
         <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="K2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="L2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="M2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -1588,39 +1567,39 @@
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="G3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="K3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="L3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="M3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -1629,31 +1608,31 @@
         <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F4" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="G4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="K4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="L4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="M4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -1670,39 +1649,39 @@
         <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H5" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="I5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J5" t="s">
         <v>5</v>
       </c>
       <c r="K5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L5" t="s">
         <v>31</v>
       </c>
-      <c r="L5" t="s">
-        <v>34</v>
-      </c>
       <c r="M5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -1711,39 +1690,39 @@
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F6" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="G6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H6" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="I6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J6" t="s">
         <v>5</v>
       </c>
       <c r="K6" t="s">
+        <v>28</v>
+      </c>
+      <c r="L6" t="s">
         <v>31</v>
       </c>
-      <c r="L6" t="s">
-        <v>34</v>
-      </c>
       <c r="M6" s="1" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -1752,39 +1731,39 @@
         <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F7" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="G7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H7" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="I7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J7" t="s">
         <v>5</v>
       </c>
       <c r="K7" t="s">
+        <v>28</v>
+      </c>
+      <c r="L7" t="s">
         <v>31</v>
       </c>
-      <c r="L7" t="s">
-        <v>34</v>
-      </c>
       <c r="M7" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -1793,39 +1772,39 @@
         <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F8" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="G8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H8" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="I8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J8" t="s">
         <v>5</v>
       </c>
       <c r="K8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L8" t="s">
         <v>31</v>
       </c>
-      <c r="L8" t="s">
-        <v>34</v>
-      </c>
       <c r="M8" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -1834,39 +1813,39 @@
         <v>5</v>
       </c>
       <c r="E9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F9" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="G9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H9" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="I9" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J9" t="s">
         <v>5</v>
       </c>
       <c r="K9" t="s">
+        <v>28</v>
+      </c>
+      <c r="L9" t="s">
         <v>31</v>
       </c>
-      <c r="L9" t="s">
-        <v>34</v>
-      </c>
       <c r="M9" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -1875,39 +1854,39 @@
         <v>5</v>
       </c>
       <c r="E10" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F10" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G10" t="s">
+        <v>28</v>
+      </c>
+      <c r="H10" t="s">
+        <v>28</v>
+      </c>
+      <c r="I10" t="s">
+        <v>28</v>
+      </c>
+      <c r="J10" t="s">
+        <v>28</v>
+      </c>
+      <c r="K10" t="s">
+        <v>28</v>
+      </c>
+      <c r="L10" t="s">
         <v>31</v>
       </c>
-      <c r="H10" t="s">
-        <v>31</v>
-      </c>
-      <c r="I10" t="s">
-        <v>31</v>
-      </c>
-      <c r="J10" t="s">
-        <v>31</v>
-      </c>
-      <c r="K10" t="s">
-        <v>31</v>
-      </c>
-      <c r="L10" t="s">
-        <v>34</v>
-      </c>
       <c r="M10" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -1916,80 +1895,80 @@
         <v>5</v>
       </c>
       <c r="E11" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F11" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G11" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" t="s">
+        <v>28</v>
+      </c>
+      <c r="I11" t="s">
+        <v>28</v>
+      </c>
+      <c r="J11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L11" t="s">
         <v>31</v>
       </c>
-      <c r="H11" t="s">
-        <v>31</v>
-      </c>
-      <c r="I11" t="s">
-        <v>31</v>
-      </c>
-      <c r="J11" t="s">
-        <v>31</v>
-      </c>
-      <c r="K11" t="s">
-        <v>31</v>
-      </c>
-      <c r="L11" t="s">
-        <v>34</v>
-      </c>
       <c r="M11" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F12" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="G12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" t="s">
+        <v>28</v>
+      </c>
+      <c r="I12" t="s">
+        <v>28</v>
+      </c>
+      <c r="J12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K12" t="s">
+        <v>27</v>
+      </c>
+      <c r="L12" t="s">
         <v>31</v>
       </c>
-      <c r="H12" t="s">
-        <v>31</v>
-      </c>
-      <c r="I12" t="s">
-        <v>31</v>
-      </c>
-      <c r="J12" t="s">
-        <v>31</v>
-      </c>
-      <c r="K12" t="s">
-        <v>31</v>
-      </c>
-      <c r="L12" t="s">
-        <v>34</v>
-      </c>
       <c r="M12" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C13" t="s">
         <v>6</v>
@@ -1998,113 +1977,31 @@
         <v>5</v>
       </c>
       <c r="E13" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" t="s">
         <v>25</v>
       </c>
-      <c r="F13" t="s">
-        <v>29</v>
-      </c>
       <c r="G13" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H13" t="s">
+        <v>28</v>
+      </c>
+      <c r="I13" t="s">
+        <v>28</v>
+      </c>
+      <c r="J13" t="s">
+        <v>28</v>
+      </c>
+      <c r="K13" t="s">
+        <v>27</v>
+      </c>
+      <c r="L13" t="s">
         <v>31</v>
       </c>
-      <c r="I13" t="s">
-        <v>31</v>
-      </c>
-      <c r="J13" t="s">
-        <v>31</v>
-      </c>
-      <c r="K13" t="s">
-        <v>30</v>
-      </c>
-      <c r="L13" t="s">
-        <v>34</v>
-      </c>
       <c r="M13" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" t="s">
-        <v>24</v>
-      </c>
-      <c r="F14" t="s">
-        <v>45</v>
-      </c>
-      <c r="G14" t="s">
-        <v>31</v>
-      </c>
-      <c r="H14" t="s">
-        <v>31</v>
-      </c>
-      <c r="I14" t="s">
-        <v>31</v>
-      </c>
-      <c r="J14" t="s">
-        <v>31</v>
-      </c>
-      <c r="K14" t="s">
-        <v>31</v>
-      </c>
-      <c r="L14" t="s">
-        <v>34</v>
-      </c>
-      <c r="M14" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" t="s">
-        <v>5</v>
-      </c>
-      <c r="E15" t="s">
-        <v>25</v>
-      </c>
-      <c r="F15" t="s">
-        <v>28</v>
-      </c>
-      <c r="G15" t="s">
-        <v>24</v>
-      </c>
-      <c r="H15" t="s">
-        <v>31</v>
-      </c>
-      <c r="I15" t="s">
-        <v>31</v>
-      </c>
-      <c r="J15" t="s">
-        <v>31</v>
-      </c>
-      <c r="K15" t="s">
-        <v>30</v>
-      </c>
-      <c r="L15" t="s">
-        <v>34</v>
-      </c>
-      <c r="M15" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more work on the things
</commit_message>
<xml_diff>
--- a/argot/working_docs/endeca_fields_to_Argot.xlsx
+++ b/argot/working_docs/endeca_fields_to_Argot.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="61">
   <si>
     <t>Element name</t>
   </si>
@@ -40,42 +40,12 @@
     <t>not indexed</t>
   </si>
   <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>Cartographic Data</t>
-  </si>
-  <si>
-    <t>Keyword</t>
-  </si>
-  <si>
-    <t>Format</t>
-  </si>
-  <si>
-    <t>LocalId</t>
-  </si>
-  <si>
-    <t>Material Details</t>
-  </si>
-  <si>
-    <t>Musical Presentation</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
-    <t>Organization</t>
-  </si>
-  <si>
     <t>PubDateSort</t>
   </si>
   <si>
-    <t>Syndetics ISBN</t>
-  </si>
-  <si>
-    <t>Syndetics_ISBN</t>
-  </si>
-  <si>
     <t>Displayed Endeca?</t>
   </si>
   <si>
@@ -88,30 +58,15 @@
     <t>y</t>
   </si>
   <si>
-    <t>n</t>
-  </si>
-  <si>
     <t>na</t>
   </si>
   <si>
     <t>Label</t>
   </si>
   <si>
-    <t>resource_type</t>
-  </si>
-  <si>
-    <t>physical_media</t>
-  </si>
-  <si>
-    <t>Facet values, but should also probably display on each record</t>
-  </si>
-  <si>
     <t>.</t>
   </si>
   <si>
-    <t>cartographic_details</t>
-  </si>
-  <si>
     <t>indexed</t>
   </si>
   <si>
@@ -136,15 +91,6 @@
     <t>defer for relevance testing</t>
   </si>
   <si>
-    <t>local_id[value]</t>
-  </si>
-  <si>
-    <t>musical_presentation_statement</t>
-  </si>
-  <si>
-    <t>organization_and_arrangement</t>
-  </si>
-  <si>
     <t>publication_year</t>
   </si>
   <si>
@@ -154,54 +100,9 @@
     <t>defer for shared records</t>
   </si>
   <si>
-    <t>syndetics_id</t>
-  </si>
-  <si>
-    <t>example: https://ingest.discovery.trln.org/record/search?id=UNCb2398669</t>
-  </si>
-  <si>
     <t>ticket</t>
   </si>
   <si>
-    <t>https://trlnmain.atlassian.net/browse/TD-462</t>
-  </si>
-  <si>
-    <t>https://trlnmain.atlassian.net/browse/TD-434</t>
-  </si>
-  <si>
-    <t>https://trlnmain.atlassian.net/browse/TD-435</t>
-  </si>
-  <si>
-    <t>https://trlnmain.atlassian.net/browse/TD-477</t>
-  </si>
-  <si>
-    <t>https://trlnmain.atlassian.net/browse/TD-478</t>
-  </si>
-  <si>
-    <t>description_details_sound</t>
-  </si>
-  <si>
-    <t>description_details_projection</t>
-  </si>
-  <si>
-    <t>description_details_video</t>
-  </si>
-  <si>
-    <t>description_details_digital_file</t>
-  </si>
-  <si>
-    <t>https://trlnmain.atlassian.net/browse/TD-479</t>
-  </si>
-  <si>
-    <t>https://trlnmain.atlassian.net/browse/TD-480</t>
-  </si>
-  <si>
-    <t>https://trlnmain.atlassian.net/browse/TD-481</t>
-  </si>
-  <si>
-    <t>https://trlnmain.atlassian.net/browse/TD-482</t>
-  </si>
-  <si>
     <t>document - done in spreadsheet.</t>
   </si>
   <si>
@@ -302,28 +203,13 @@
   </si>
   <si>
     <t>Display notes</t>
-  </si>
-  <si>
-    <t>Other details &gt; (material description cluster) &gt; Video details:</t>
-  </si>
-  <si>
-    <t>Other details &gt; (material description cluster) &gt; Sound details:</t>
-  </si>
-  <si>
-    <t>Other details &gt; (material description cluster) &gt; Projection details:</t>
-  </si>
-  <si>
-    <t>Other details &gt; (material description cluster) &gt; Digital file details:</t>
-  </si>
-  <si>
-    <t>Other details &gt; (material description cluster) &gt; Cartographic details:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -454,14 +340,6 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -764,7 +642,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -807,11 +685,9 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -828,7 +704,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -862,7 +738,6 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -931,8 +806,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="endecafields" displayName="endecafields" ref="A1:M13" totalsRowShown="0">
-  <autoFilter ref="A1:M13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="endecafields" displayName="endecafields" ref="A1:M2" totalsRowShown="0">
+  <autoFilter ref="A1:M2"/>
   <tableColumns count="13">
     <tableColumn id="1" name="Element name"/>
     <tableColumn id="2" name="Endeca dmod name"/>
@@ -1224,221 +1099,221 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.42578125" customWidth="1"/>
-    <col min="2" max="2" width="65.28515625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="65.28515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="B1" s="6"/>
+      <c r="A1" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="5"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>64</v>
+        <v>30</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>65</v>
+      <c r="B4" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>66</v>
+      <c r="B5" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>67</v>
+      <c r="B6" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>68</v>
+      <c r="B7" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>69</v>
+      <c r="A8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>70</v>
+      <c r="A9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>71</v>
+      <c r="A10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>72</v>
+      <c r="A11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>73</v>
+      <c r="A12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>75</v>
+      <c r="A13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>76</v>
+      <c r="A14" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>77</v>
+      <c r="A15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>78</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>79</v>
+        <v>45</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>80</v>
+      <c r="A19" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>81</v>
+      <c r="A20" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>82</v>
+      <c r="A21" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>83</v>
+      <c r="A22" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>84</v>
+      <c r="A23" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>85</v>
+      <c r="A24" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>87</v>
+      <c r="A25" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>86</v>
+      <c r="A26" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>88</v>
+      <c r="A27" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>89</v>
+      <c r="A28" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>90</v>
+      <c r="A29" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>91</v>
+      <c r="A30" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1455,10 +1330,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1485,532 +1360,78 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="F1" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="G1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="H1" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="I1" t="s">
-        <v>93</v>
+        <v>60</v>
       </c>
       <c r="J1" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="K1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="L1" t="s">
-        <v>74</v>
+        <v>41</v>
       </c>
       <c r="M1" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="G2" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="H2" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="I2" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="J2" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="L2" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="M2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J3" t="s">
-        <v>28</v>
-      </c>
-      <c r="K3" t="s">
-        <v>42</v>
-      </c>
-      <c r="L3" t="s">
-        <v>34</v>
-      </c>
-      <c r="M3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G4" t="s">
-        <v>28</v>
-      </c>
-      <c r="H4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J4" t="s">
-        <v>28</v>
-      </c>
-      <c r="K4" t="s">
-        <v>45</v>
-      </c>
-      <c r="L4" t="s">
-        <v>34</v>
-      </c>
-      <c r="M4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" t="s">
-        <v>98</v>
-      </c>
-      <c r="I5" t="s">
-        <v>28</v>
-      </c>
-      <c r="J5" t="s">
-        <v>5</v>
-      </c>
-      <c r="K5" t="s">
-        <v>28</v>
-      </c>
-      <c r="L5" t="s">
-        <v>31</v>
-      </c>
-      <c r="M5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" t="s">
-        <v>55</v>
-      </c>
-      <c r="G6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H6" t="s">
-        <v>97</v>
-      </c>
-      <c r="I6" t="s">
-        <v>28</v>
-      </c>
-      <c r="J6" t="s">
-        <v>5</v>
-      </c>
-      <c r="K6" t="s">
-        <v>28</v>
-      </c>
-      <c r="L6" t="s">
-        <v>31</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" t="s">
-        <v>53</v>
-      </c>
-      <c r="G7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H7" t="s">
-        <v>96</v>
-      </c>
-      <c r="I7" t="s">
-        <v>28</v>
-      </c>
-      <c r="J7" t="s">
-        <v>5</v>
-      </c>
-      <c r="K7" t="s">
-        <v>28</v>
-      </c>
-      <c r="L7" t="s">
-        <v>31</v>
-      </c>
-      <c r="M7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" t="s">
-        <v>52</v>
-      </c>
-      <c r="G8" t="s">
-        <v>21</v>
-      </c>
-      <c r="H8" t="s">
-        <v>95</v>
-      </c>
-      <c r="I8" t="s">
-        <v>28</v>
-      </c>
-      <c r="J8" t="s">
-        <v>5</v>
-      </c>
-      <c r="K8" t="s">
-        <v>28</v>
-      </c>
-      <c r="L8" t="s">
-        <v>31</v>
-      </c>
-      <c r="M8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" t="s">
-        <v>54</v>
-      </c>
-      <c r="G9" t="s">
-        <v>21</v>
-      </c>
-      <c r="H9" t="s">
-        <v>94</v>
-      </c>
-      <c r="I9" t="s">
-        <v>28</v>
-      </c>
-      <c r="J9" t="s">
-        <v>5</v>
-      </c>
-      <c r="K9" t="s">
-        <v>28</v>
-      </c>
-      <c r="L9" t="s">
-        <v>31</v>
-      </c>
-      <c r="M9" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F10" t="s">
-        <v>39</v>
-      </c>
-      <c r="G10" t="s">
-        <v>28</v>
-      </c>
-      <c r="H10" t="s">
-        <v>28</v>
-      </c>
-      <c r="I10" t="s">
-        <v>28</v>
-      </c>
-      <c r="J10" t="s">
-        <v>28</v>
-      </c>
-      <c r="K10" t="s">
-        <v>28</v>
-      </c>
-      <c r="L10" t="s">
-        <v>31</v>
-      </c>
-      <c r="M10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
         <v>14</v>
       </c>
-      <c r="B11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" t="s">
-        <v>40</v>
-      </c>
-      <c r="G11" t="s">
-        <v>28</v>
-      </c>
-      <c r="H11" t="s">
-        <v>28</v>
-      </c>
-      <c r="I11" t="s">
-        <v>28</v>
-      </c>
-      <c r="J11" t="s">
-        <v>28</v>
-      </c>
-      <c r="K11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L11" t="s">
-        <v>31</v>
-      </c>
-      <c r="M11" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12" t="s">
-        <v>26</v>
-      </c>
-      <c r="G12" t="s">
-        <v>21</v>
-      </c>
-      <c r="H12" t="s">
-        <v>28</v>
-      </c>
-      <c r="I12" t="s">
-        <v>28</v>
-      </c>
-      <c r="J12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K12" t="s">
-        <v>27</v>
-      </c>
-      <c r="L12" t="s">
-        <v>31</v>
-      </c>
-      <c r="M12" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" t="s">
-        <v>25</v>
-      </c>
-      <c r="G13" t="s">
-        <v>21</v>
-      </c>
-      <c r="H13" t="s">
-        <v>28</v>
-      </c>
-      <c r="I13" t="s">
-        <v>28</v>
-      </c>
-      <c r="J13" t="s">
-        <v>28</v>
-      </c>
-      <c r="K13" t="s">
-        <v>27</v>
-      </c>
-      <c r="L13" t="s">
-        <v>31</v>
-      </c>
-      <c r="M13" t="s">
-        <v>48</v>
-      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="M6" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>